<commit_message>
Add /api/theme-attributes endpoint for PRD
</commit_message>
<xml_diff>
--- a/Genel Tema.xlsx
+++ b/Genel Tema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaank\Downloads\IpekyolTema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9241D-0282-4964-8FC3-79BC882B2963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6638963F-53F4-4789-8C4D-ED4D0F9CE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <definedName name="DışVeri_2" localSheetId="1" hidden="1">Sayfa2!$AI$1:$AL$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2842,7 +2843,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -2882,7 +2883,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="41" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="41" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="41" applyNumberFormat="1"/>
   </cellXfs>
@@ -7248,8 +7248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC03FFC2-59C1-4D40-8D76-DB01FBACC3CE}">
   <dimension ref="A1:BA103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7257,6 +7257,7 @@
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="31.5">
@@ -13105,7 +13106,7 @@
       <c r="D54" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="E54" s="21">
+      <c r="E54" s="20">
         <v>46023</v>
       </c>
       <c r="F54" s="19" t="s">
@@ -13138,10 +13139,10 @@
       <c r="O54" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P54" s="20" t="s">
+      <c r="P54" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="Q54" s="20" t="s">
+      <c r="Q54" s="19" t="s">
         <v>235</v>
       </c>
       <c r="R54" s="19" t="s">
@@ -13168,10 +13169,10 @@
       <c r="Y54" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z54" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA54" s="20" t="s">
+      <c r="Z54" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA54" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD54" s="10">
@@ -13215,7 +13216,7 @@
       <c r="D55" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="E55" s="21">
+      <c r="E55" s="20">
         <v>46023</v>
       </c>
       <c r="F55" s="19" t="s">
@@ -13248,10 +13249,10 @@
       <c r="O55" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q55" s="20" t="s">
+      <c r="P55" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q55" s="19" t="s">
         <v>178</v>
       </c>
       <c r="R55" s="19" t="s">
@@ -13278,10 +13279,10 @@
       <c r="Y55" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z55" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA55" s="20" t="s">
+      <c r="Z55" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA55" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD55" s="11">
@@ -13325,7 +13326,7 @@
       <c r="D56" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="E56" s="21">
+      <c r="E56" s="20">
         <v>46023</v>
       </c>
       <c r="F56" s="19" t="s">
@@ -13358,10 +13359,10 @@
       <c r="O56" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P56" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q56" s="20" t="s">
+      <c r="P56" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q56" s="19" t="s">
         <v>179</v>
       </c>
       <c r="R56" s="19" t="s">
@@ -13388,10 +13389,10 @@
       <c r="Y56" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z56" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA56" s="20" t="s">
+      <c r="Z56" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA56" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD56" s="10">
@@ -13435,7 +13436,7 @@
       <c r="D57" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E57" s="20">
         <v>46023</v>
       </c>
       <c r="F57" s="19" t="s">
@@ -13468,10 +13469,10 @@
       <c r="O57" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P57" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q57" s="20" t="s">
+      <c r="P57" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q57" s="19" t="s">
         <v>181</v>
       </c>
       <c r="R57" s="19" t="s">
@@ -13498,10 +13499,10 @@
       <c r="Y57" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z57" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA57" s="20" t="s">
+      <c r="Z57" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA57" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD57" s="11">
@@ -13545,7 +13546,7 @@
       <c r="D58" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="E58" s="21">
+      <c r="E58" s="20">
         <v>46023</v>
       </c>
       <c r="F58" s="19" t="s">
@@ -13578,10 +13579,10 @@
       <c r="O58" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P58" s="20" t="s">
+      <c r="P58" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="Q58" s="20" t="s">
+      <c r="Q58" s="19" t="s">
         <v>182</v>
       </c>
       <c r="R58" s="19" t="s">
@@ -13608,10 +13609,10 @@
       <c r="Y58" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z58" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA58" s="20" t="s">
+      <c r="Z58" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA58" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD58" s="10">
@@ -13655,7 +13656,7 @@
       <c r="D59" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="E59" s="21">
+      <c r="E59" s="20">
         <v>46023</v>
       </c>
       <c r="F59" s="19" t="s">
@@ -13688,10 +13689,10 @@
       <c r="O59" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P59" s="20" t="s">
+      <c r="P59" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="Q59" s="20" t="s">
+      <c r="Q59" s="19" t="s">
         <v>183</v>
       </c>
       <c r="R59" s="19" t="s">
@@ -13718,10 +13719,10 @@
       <c r="Y59" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z59" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA59" s="20" t="s">
+      <c r="Z59" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA59" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD59" s="11">
@@ -13765,7 +13766,7 @@
       <c r="D60" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="E60" s="21">
+      <c r="E60" s="20">
         <v>46023</v>
       </c>
       <c r="F60" s="19" t="s">
@@ -13798,10 +13799,10 @@
       <c r="O60" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P60" s="20" t="s">
+      <c r="P60" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="Q60" s="20" t="s">
+      <c r="Q60" s="19" t="s">
         <v>184</v>
       </c>
       <c r="R60" s="19" t="s">
@@ -13828,10 +13829,10 @@
       <c r="Y60" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z60" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA60" s="20" t="s">
+      <c r="Z60" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA60" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD60" s="10">
@@ -13875,7 +13876,7 @@
       <c r="D61" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="E61" s="21">
+      <c r="E61" s="20">
         <v>46023</v>
       </c>
       <c r="F61" s="19" t="s">
@@ -13908,10 +13909,10 @@
       <c r="O61" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P61" s="20" t="s">
+      <c r="P61" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Q61" s="20" t="s">
+      <c r="Q61" s="19" t="s">
         <v>187</v>
       </c>
       <c r="R61" s="19" t="s">
@@ -13938,10 +13939,10 @@
       <c r="Y61" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z61" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA61" s="20" t="s">
+      <c r="Z61" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA61" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD61" s="11">
@@ -13985,7 +13986,7 @@
       <c r="D62" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="E62" s="21">
+      <c r="E62" s="20">
         <v>46023</v>
       </c>
       <c r="F62" s="19" t="s">
@@ -14018,10 +14019,10 @@
       <c r="O62" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P62" s="20" t="s">
+      <c r="P62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="Q62" s="20" t="s">
+      <c r="Q62" s="19" t="s">
         <v>188</v>
       </c>
       <c r="R62" s="19" t="s">
@@ -14048,10 +14049,10 @@
       <c r="Y62" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z62" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA62" s="20" t="s">
+      <c r="Z62" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA62" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD62" s="10">
@@ -14095,7 +14096,7 @@
       <c r="D63" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="E63" s="21">
+      <c r="E63" s="20">
         <v>46023</v>
       </c>
       <c r="F63" s="19" t="s">
@@ -14128,10 +14129,10 @@
       <c r="O63" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P63" s="20" t="s">
+      <c r="P63" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="Q63" s="20" t="s">
+      <c r="Q63" s="19" t="s">
         <v>189</v>
       </c>
       <c r="R63" s="19" t="s">
@@ -14158,10 +14159,10 @@
       <c r="Y63" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z63" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA63" s="20" t="s">
+      <c r="Z63" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA63" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD63" s="11">
@@ -14205,7 +14206,7 @@
       <c r="D64" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="E64" s="21">
+      <c r="E64" s="20">
         <v>46023</v>
       </c>
       <c r="F64" s="19" t="s">
@@ -14238,10 +14239,10 @@
       <c r="O64" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P64" s="20" t="s">
+      <c r="P64" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="Q64" s="20" t="s">
+      <c r="Q64" s="19" t="s">
         <v>237</v>
       </c>
       <c r="R64" s="19" t="s">
@@ -14268,10 +14269,10 @@
       <c r="Y64" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z64" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA64" s="20" t="s">
+      <c r="Z64" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA64" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD64" s="10">
@@ -14315,7 +14316,7 @@
       <c r="D65" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="E65" s="21">
+      <c r="E65" s="20">
         <v>46023</v>
       </c>
       <c r="F65" s="19" t="s">
@@ -14348,10 +14349,10 @@
       <c r="O65" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P65" s="20" t="s">
+      <c r="P65" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="Q65" s="20" t="s">
+      <c r="Q65" s="19" t="s">
         <v>239</v>
       </c>
       <c r="R65" s="19" t="s">
@@ -14378,10 +14379,10 @@
       <c r="Y65" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z65" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA65" s="20" t="s">
+      <c r="Z65" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA65" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD65" s="11">
@@ -14425,7 +14426,7 @@
       <c r="D66" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="E66" s="21">
+      <c r="E66" s="20">
         <v>46023</v>
       </c>
       <c r="F66" s="19" t="s">
@@ -14458,10 +14459,10 @@
       <c r="O66" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P66" s="20" t="s">
+      <c r="P66" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="Q66" s="20" t="s">
+      <c r="Q66" s="19" t="s">
         <v>241</v>
       </c>
       <c r="R66" s="19" t="s">
@@ -14488,10 +14489,10 @@
       <c r="Y66" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z66" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA66" s="20" t="s">
+      <c r="Z66" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA66" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD66" s="10">
@@ -14535,7 +14536,7 @@
       <c r="D67" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="E67" s="21">
+      <c r="E67" s="20">
         <v>46023</v>
       </c>
       <c r="F67" s="19" t="s">
@@ -14568,10 +14569,10 @@
       <c r="O67" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P67" s="20" t="s">
+      <c r="P67" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Q67" s="20" t="s">
+      <c r="Q67" s="19" t="s">
         <v>242</v>
       </c>
       <c r="R67" s="19" t="s">
@@ -14598,10 +14599,10 @@
       <c r="Y67" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z67" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA67" s="20" t="s">
+      <c r="Z67" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA67" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD67" s="11">
@@ -14645,7 +14646,7 @@
       <c r="D68" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="E68" s="21">
+      <c r="E68" s="20">
         <v>46023</v>
       </c>
       <c r="F68" s="19" t="s">
@@ -14678,10 +14679,10 @@
       <c r="O68" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P68" s="20" t="s">
+      <c r="P68" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="Q68" s="20" t="s">
+      <c r="Q68" s="19" t="s">
         <v>244</v>
       </c>
       <c r="R68" s="19" t="s">
@@ -14708,10 +14709,10 @@
       <c r="Y68" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z68" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA68" s="20" t="s">
+      <c r="Z68" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA68" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD68" s="10">
@@ -14755,7 +14756,7 @@
       <c r="D69" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="E69" s="21">
+      <c r="E69" s="20">
         <v>46023</v>
       </c>
       <c r="F69" s="19" t="s">
@@ -14788,10 +14789,10 @@
       <c r="O69" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P69" s="20" t="s">
+      <c r="P69" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="Q69" s="20" t="s">
+      <c r="Q69" s="19" t="s">
         <v>245</v>
       </c>
       <c r="R69" s="19" t="s">
@@ -14818,10 +14819,10 @@
       <c r="Y69" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z69" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA69" s="20" t="s">
+      <c r="Z69" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA69" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD69" s="11">
@@ -14865,7 +14866,7 @@
       <c r="D70" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="E70" s="21">
+      <c r="E70" s="20">
         <v>46023</v>
       </c>
       <c r="F70" s="19" t="s">
@@ -14898,10 +14899,10 @@
       <c r="O70" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P70" s="20" t="s">
+      <c r="P70" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q70" s="20" t="s">
+      <c r="Q70" s="19" t="s">
         <v>246</v>
       </c>
       <c r="R70" s="19" t="s">
@@ -14928,10 +14929,10 @@
       <c r="Y70" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z70" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA70" s="20" t="s">
+      <c r="Z70" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA70" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD70" s="10">
@@ -14975,7 +14976,7 @@
       <c r="D71" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="E71" s="21">
+      <c r="E71" s="20">
         <v>46023</v>
       </c>
       <c r="F71" s="19" t="s">
@@ -15008,10 +15009,10 @@
       <c r="O71" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P71" s="20" t="s">
+      <c r="P71" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="Q71" s="20" t="s">
+      <c r="Q71" s="19" t="s">
         <v>248</v>
       </c>
       <c r="R71" s="19" t="s">
@@ -15038,10 +15039,10 @@
       <c r="Y71" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z71" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA71" s="20" t="s">
+      <c r="Z71" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA71" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD71" s="11">
@@ -15085,7 +15086,7 @@
       <c r="D72" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E72" s="21">
+      <c r="E72" s="20">
         <v>46023</v>
       </c>
       <c r="F72" s="19" t="s">
@@ -15118,10 +15119,10 @@
       <c r="O72" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P72" s="20" t="s">
+      <c r="P72" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="Q72" s="20" t="s">
+      <c r="Q72" s="19" t="s">
         <v>250</v>
       </c>
       <c r="R72" s="19" t="s">
@@ -15148,10 +15149,10 @@
       <c r="Y72" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z72" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA72" s="20" t="s">
+      <c r="Z72" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA72" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD72" s="10">
@@ -15195,7 +15196,7 @@
       <c r="D73" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="E73" s="21">
+      <c r="E73" s="20">
         <v>46023</v>
       </c>
       <c r="F73" s="19" t="s">
@@ -15228,10 +15229,10 @@
       <c r="O73" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P73" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q73" s="20" t="s">
+      <c r="P73" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q73" s="19" t="s">
         <v>178</v>
       </c>
       <c r="R73" s="19" t="s">
@@ -15258,10 +15259,10 @@
       <c r="Y73" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z73" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA73" s="20" t="s">
+      <c r="Z73" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA73" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD73" s="11">
@@ -15305,7 +15306,7 @@
       <c r="D74" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="E74" s="21">
+      <c r="E74" s="20">
         <v>46023</v>
       </c>
       <c r="F74" s="19" t="s">
@@ -15338,10 +15339,10 @@
       <c r="O74" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P74" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q74" s="20" t="s">
+      <c r="P74" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q74" s="19" t="s">
         <v>179</v>
       </c>
       <c r="R74" s="19" t="s">
@@ -15368,10 +15369,10 @@
       <c r="Y74" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z74" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA74" s="20" t="s">
+      <c r="Z74" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA74" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD74" s="10">
@@ -15415,7 +15416,7 @@
       <c r="D75" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="E75" s="21">
+      <c r="E75" s="20">
         <v>46023</v>
       </c>
       <c r="F75" s="19" t="s">
@@ -15448,10 +15449,10 @@
       <c r="O75" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P75" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q75" s="20" t="s">
+      <c r="P75" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="19" t="s">
         <v>181</v>
       </c>
       <c r="R75" s="19" t="s">
@@ -15478,10 +15479,10 @@
       <c r="Y75" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z75" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA75" s="20" t="s">
+      <c r="Z75" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA75" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD75" s="11">
@@ -15525,7 +15526,7 @@
       <c r="D76" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="E76" s="21">
+      <c r="E76" s="20">
         <v>46023</v>
       </c>
       <c r="F76" s="19" t="s">
@@ -15558,10 +15559,10 @@
       <c r="O76" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P76" s="20" t="s">
+      <c r="P76" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Q76" s="20" t="s">
+      <c r="Q76" s="19" t="s">
         <v>187</v>
       </c>
       <c r="R76" s="19" t="s">
@@ -15588,10 +15589,10 @@
       <c r="Y76" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z76" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA76" s="20" t="s">
+      <c r="Z76" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA76" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD76" s="10">
@@ -15635,7 +15636,7 @@
       <c r="D77" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="E77" s="21">
+      <c r="E77" s="20">
         <v>46023</v>
       </c>
       <c r="F77" s="19" t="s">
@@ -15668,10 +15669,10 @@
       <c r="O77" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P77" s="20" t="s">
+      <c r="P77" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="Q77" s="20" t="s">
+      <c r="Q77" s="19" t="s">
         <v>237</v>
       </c>
       <c r="R77" s="19" t="s">
@@ -15698,10 +15699,10 @@
       <c r="Y77" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z77" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA77" s="20" t="s">
+      <c r="Z77" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA77" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD77" s="11">
@@ -15745,7 +15746,7 @@
       <c r="D78" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="E78" s="21">
+      <c r="E78" s="20">
         <v>46023</v>
       </c>
       <c r="F78" s="19" t="s">
@@ -15778,10 +15779,10 @@
       <c r="O78" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P78" s="20" t="s">
+      <c r="P78" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="Q78" s="20" t="s">
+      <c r="Q78" s="19" t="s">
         <v>239</v>
       </c>
       <c r="R78" s="19" t="s">
@@ -15808,10 +15809,10 @@
       <c r="Y78" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z78" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA78" s="20" t="s">
+      <c r="Z78" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA78" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD78" s="10">
@@ -15855,7 +15856,7 @@
       <c r="D79" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="E79" s="21">
+      <c r="E79" s="20">
         <v>46023</v>
       </c>
       <c r="F79" s="19" t="s">
@@ -15888,10 +15889,10 @@
       <c r="O79" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P79" s="20" t="s">
+      <c r="P79" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="Q79" s="20" t="s">
+      <c r="Q79" s="19" t="s">
         <v>241</v>
       </c>
       <c r="R79" s="19" t="s">
@@ -15918,10 +15919,10 @@
       <c r="Y79" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z79" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA79" s="20" t="s">
+      <c r="Z79" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA79" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD79" s="11">
@@ -15965,7 +15966,7 @@
       <c r="D80" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="E80" s="21">
+      <c r="E80" s="20">
         <v>46023</v>
       </c>
       <c r="F80" s="19" t="s">
@@ -15998,10 +15999,10 @@
       <c r="O80" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P80" s="20" t="s">
+      <c r="P80" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q80" s="20" t="s">
+      <c r="Q80" s="19" t="s">
         <v>246</v>
       </c>
       <c r="R80" s="19" t="s">
@@ -16028,10 +16029,10 @@
       <c r="Y80" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z80" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA80" s="20" t="s">
+      <c r="Z80" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA80" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD80" s="10">
@@ -16075,7 +16076,7 @@
       <c r="D81" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="E81" s="21">
+      <c r="E81" s="20">
         <v>46023</v>
       </c>
       <c r="F81" s="19" t="s">
@@ -16108,10 +16109,10 @@
       <c r="O81" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P81" s="20" t="s">
+      <c r="P81" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="Q81" s="20" t="s">
+      <c r="Q81" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R81" s="19" t="s">
@@ -16138,10 +16139,10 @@
       <c r="Y81" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="Z81" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA81" s="20" t="s">
+      <c r="Z81" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA81" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD81" s="11">
@@ -16185,7 +16186,7 @@
       <c r="D82" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="E82" s="21">
+      <c r="E82" s="20">
         <v>1</v>
       </c>
       <c r="F82" s="19" t="s">
@@ -16218,10 +16219,10 @@
       <c r="O82" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P82" s="20" t="s">
+      <c r="P82" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="Q82" s="20" t="s">
+      <c r="Q82" s="19" t="s">
         <v>254</v>
       </c>
       <c r="R82" s="19" t="s">
@@ -16248,10 +16249,10 @@
       <c r="Y82" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z82" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA82" s="20" t="s">
+      <c r="Z82" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA82" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD82" s="10">
@@ -16295,7 +16296,7 @@
       <c r="D83" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="E83" s="21">
+      <c r="E83" s="20">
         <v>46192</v>
       </c>
       <c r="F83" s="19" t="s">
@@ -16328,10 +16329,10 @@
       <c r="O83" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P83" s="20" t="s">
+      <c r="P83" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="Q83" s="20" t="s">
+      <c r="Q83" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R83" s="19" t="s">
@@ -16358,10 +16359,10 @@
       <c r="Y83" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="Z83" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA83" s="20" t="s">
+      <c r="Z83" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA83" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD83" s="11">
@@ -16405,7 +16406,7 @@
       <c r="D84" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="E84" s="21">
+      <c r="E84" s="20">
         <v>46192</v>
       </c>
       <c r="F84" s="19" t="s">
@@ -16438,10 +16439,10 @@
       <c r="O84" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P84" s="20" t="s">
+      <c r="P84" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="Q84" s="20" t="s">
+      <c r="Q84" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R84" s="19" t="s">
@@ -16468,10 +16469,10 @@
       <c r="Y84" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="Z84" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA84" s="20" t="s">
+      <c r="Z84" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA84" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD84" s="10">
@@ -16515,7 +16516,7 @@
       <c r="D85" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="E85" s="21">
+      <c r="E85" s="20">
         <v>46192</v>
       </c>
       <c r="F85" s="19" t="s">
@@ -16548,10 +16549,10 @@
       <c r="O85" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P85" s="20" t="s">
+      <c r="P85" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="Q85" s="20" t="s">
+      <c r="Q85" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R85" s="19" t="s">
@@ -16578,10 +16579,10 @@
       <c r="Y85" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="Z85" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA85" s="20" t="s">
+      <c r="Z85" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA85" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD85" s="11">
@@ -16625,7 +16626,7 @@
       <c r="D86" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="E86" s="21">
+      <c r="E86" s="20">
         <v>46192</v>
       </c>
       <c r="F86" s="19" t="s">
@@ -16658,10 +16659,10 @@
       <c r="O86" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P86" s="20" t="s">
+      <c r="P86" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="Q86" s="20" t="s">
+      <c r="Q86" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R86" s="19" t="s">
@@ -16688,10 +16689,10 @@
       <c r="Y86" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="Z86" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA86" s="20" t="s">
+      <c r="Z86" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA86" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD86" s="10">
@@ -16735,7 +16736,7 @@
       <c r="D87" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="E87" s="21">
+      <c r="E87" s="20">
         <v>46023</v>
       </c>
       <c r="F87" s="19" t="s">
@@ -16768,10 +16769,10 @@
       <c r="O87" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P87" s="20" t="s">
+      <c r="P87" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="Q87" s="20" t="s">
+      <c r="Q87" s="19" t="s">
         <v>182</v>
       </c>
       <c r="R87" s="19" t="s">
@@ -16798,10 +16799,10 @@
       <c r="Y87" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z87" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA87" s="20" t="s">
+      <c r="Z87" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA87" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD87" s="11">
@@ -16845,7 +16846,7 @@
       <c r="D88" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="E88" s="21">
+      <c r="E88" s="20">
         <v>46023</v>
       </c>
       <c r="F88" s="19" t="s">
@@ -16878,10 +16879,10 @@
       <c r="O88" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P88" s="20" t="s">
+      <c r="P88" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="Q88" s="20" t="s">
+      <c r="Q88" s="19" t="s">
         <v>184</v>
       </c>
       <c r="R88" s="19" t="s">
@@ -16908,10 +16909,10 @@
       <c r="Y88" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z88" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA88" s="20" t="s">
+      <c r="Z88" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA88" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD88" s="10">
@@ -16955,7 +16956,7 @@
       <c r="D89" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="E89" s="21">
+      <c r="E89" s="20">
         <v>46023</v>
       </c>
       <c r="F89" s="19" t="s">
@@ -16988,10 +16989,10 @@
       <c r="O89" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P89" s="20" t="s">
+      <c r="P89" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="Q89" s="20" t="s">
+      <c r="Q89" s="19" t="s">
         <v>245</v>
       </c>
       <c r="R89" s="19" t="s">
@@ -17018,10 +17019,10 @@
       <c r="Y89" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z89" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA89" s="20" t="s">
+      <c r="Z89" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA89" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD89" s="11">
@@ -17065,7 +17066,7 @@
       <c r="D90" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="E90" s="21">
+      <c r="E90" s="20">
         <v>46023</v>
       </c>
       <c r="F90" s="19" t="s">
@@ -17098,10 +17099,10 @@
       <c r="O90" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P90" s="20" t="s">
+      <c r="P90" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="Q90" s="20" t="s">
+      <c r="Q90" s="19" t="s">
         <v>250</v>
       </c>
       <c r="R90" s="19" t="s">
@@ -17128,10 +17129,10 @@
       <c r="Y90" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z90" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA90" s="20" t="s">
+      <c r="Z90" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA90" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD90" s="10">
@@ -17175,7 +17176,7 @@
       <c r="D91" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="E91" s="21">
+      <c r="E91" s="20">
         <v>46023</v>
       </c>
       <c r="F91" s="19" t="s">
@@ -17208,10 +17209,10 @@
       <c r="O91" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P91" s="20" t="s">
+      <c r="P91" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="Q91" s="20" t="s">
+      <c r="Q91" s="19" t="s">
         <v>183</v>
       </c>
       <c r="R91" s="19" t="s">
@@ -17238,10 +17239,10 @@
       <c r="Y91" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Z91" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA91" s="20" t="s">
+      <c r="Z91" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA91" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD91" s="11">
@@ -17285,7 +17286,7 @@
       <c r="D92" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="E92" s="21">
+      <c r="E92" s="20">
         <v>1</v>
       </c>
       <c r="F92" s="19" t="s">
@@ -17318,10 +17319,10 @@
       <c r="O92" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P92" s="20" t="s">
+      <c r="P92" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="Q92" s="20" t="s">
+      <c r="Q92" s="19" t="s">
         <v>254</v>
       </c>
       <c r="R92" s="19" t="s">
@@ -17348,10 +17349,10 @@
       <c r="Y92" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z92" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA92" s="20" t="s">
+      <c r="Z92" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA92" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD92" s="10">
@@ -17395,7 +17396,7 @@
       <c r="D93" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="E93" s="21">
+      <c r="E93" s="20">
         <v>1</v>
       </c>
       <c r="F93" s="19" t="s">
@@ -17428,10 +17429,10 @@
       <c r="O93" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P93" s="20" t="s">
+      <c r="P93" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="Q93" s="20" t="s">
+      <c r="Q93" s="19" t="s">
         <v>254</v>
       </c>
       <c r="R93" s="19" t="s">
@@ -17458,10 +17459,10 @@
       <c r="Y93" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z93" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA93" s="20" t="s">
+      <c r="Z93" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA93" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD93" s="11">
@@ -17505,7 +17506,7 @@
       <c r="D94" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="E94" s="21">
+      <c r="E94" s="20">
         <v>1</v>
       </c>
       <c r="F94" s="19" t="s">
@@ -17538,10 +17539,10 @@
       <c r="O94" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P94" s="20" t="s">
+      <c r="P94" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="Q94" s="20" t="s">
+      <c r="Q94" s="19" t="s">
         <v>254</v>
       </c>
       <c r="R94" s="19" t="s">
@@ -17568,10 +17569,10 @@
       <c r="Y94" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z94" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA94" s="20" t="s">
+      <c r="Z94" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA94" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD94" s="10">
@@ -17615,7 +17616,7 @@
       <c r="D95" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="E95" s="21">
+      <c r="E95" s="20">
         <v>1</v>
       </c>
       <c r="F95" s="19" t="s">
@@ -17648,10 +17649,10 @@
       <c r="O95" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P95" s="20" t="s">
+      <c r="P95" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="Q95" s="20" t="s">
+      <c r="Q95" s="19" t="s">
         <v>254</v>
       </c>
       <c r="R95" s="19" t="s">
@@ -17678,10 +17679,10 @@
       <c r="Y95" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z95" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA95" s="20" t="s">
+      <c r="Z95" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA95" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD95" s="11">
@@ -17725,7 +17726,7 @@
       <c r="D96" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="E96" s="21">
+      <c r="E96" s="20">
         <v>46023</v>
       </c>
       <c r="F96" s="19" t="s">
@@ -17758,10 +17759,10 @@
       <c r="O96" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P96" s="20" t="s">
+      <c r="P96" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="Q96" s="20" t="s">
+      <c r="Q96" s="19" t="s">
         <v>235</v>
       </c>
       <c r="R96" s="19" t="s">
@@ -17788,10 +17789,10 @@
       <c r="Y96" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z96" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA96" s="20" t="s">
+      <c r="Z96" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA96" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD96" s="10">
@@ -17835,7 +17836,7 @@
       <c r="D97" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="E97" s="21">
+      <c r="E97" s="20">
         <v>1</v>
       </c>
       <c r="F97" s="19" t="s">
@@ -17868,10 +17869,10 @@
       <c r="O97" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P97" s="20" t="s">
+      <c r="P97" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="Q97" s="20" t="s">
+      <c r="Q97" s="19" t="s">
         <v>235</v>
       </c>
       <c r="R97" s="19" t="s">
@@ -17898,10 +17899,10 @@
       <c r="Y97" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="Z97" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA97" s="20" t="s">
+      <c r="Z97" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA97" s="19" t="s">
         <v>63</v>
       </c>
       <c r="AD97" s="11">
@@ -18037,7 +18038,7 @@
       <c r="AD103" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="AE103" s="21">
+      <c r="AE103" s="20">
         <v>46023</v>
       </c>
       <c r="AF103" s="19" t="s">
@@ -18070,10 +18071,10 @@
       <c r="AO103" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AP103" s="20" t="s">
+      <c r="AP103" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="AQ103" s="20" t="s">
+      <c r="AQ103" s="19" t="s">
         <v>235</v>
       </c>
       <c r="AR103" s="19" t="s">
@@ -18100,10 +18101,10 @@
       <c r="AY103" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AZ103" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="BA103" s="20" t="s">
+      <c r="AZ103" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA103" s="19" t="s">
         <v>63</v>
       </c>
     </row>
@@ -18130,7 +18131,7 @@
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -18416,7 +18417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2F3C16-8AFF-41ED-86B4-5C1724269C84}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -20583,16 +20584,16 @@
       <c r="A54" t="s">
         <v>712</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="20" t="s">
+      <c r="D54" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E54" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F54">
@@ -20601,22 +20602,22 @@
       <c r="G54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I54" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J54" s="20" t="s">
+      <c r="I54" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K54" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L54" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M54" s="20" t="s">
+      <c r="L54" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20624,16 +20625,16 @@
       <c r="A55" t="s">
         <v>706</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E55" s="20" t="s">
+      <c r="D55" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F55">
@@ -20642,22 +20643,22 @@
       <c r="G55" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J55" s="20" t="s">
+      <c r="H55" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J55" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K55" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M55" s="20" t="s">
+      <c r="L55" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M55" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20665,16 +20666,16 @@
       <c r="A56" t="s">
         <v>710</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F56">
@@ -20683,22 +20684,22 @@
       <c r="G56" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H56" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I56" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J56" s="20" t="s">
+      <c r="H56" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K56" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L56" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M56" s="20" t="s">
+      <c r="L56" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M56" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20706,16 +20707,16 @@
       <c r="A57" t="s">
         <v>708</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E57" s="20" t="s">
+      <c r="D57" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F57">
@@ -20724,22 +20725,22 @@
       <c r="G57" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H57" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I57" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J57" s="20" t="s">
+      <c r="H57" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K57" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L57" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M57" s="20" t="s">
+      <c r="L57" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M57" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20747,16 +20748,16 @@
       <c r="A58" t="s">
         <v>704</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F58">
@@ -20765,22 +20766,22 @@
       <c r="G58" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H58" s="20" t="s">
+      <c r="H58" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I58" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J58" s="20" t="s">
+      <c r="I58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J58" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K58" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M58" s="20" t="s">
+      <c r="L58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20788,16 +20789,16 @@
       <c r="A59" t="s">
         <v>702</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E59" s="20" t="s">
+      <c r="D59" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F59">
@@ -20806,22 +20807,22 @@
       <c r="G59" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H59" s="20" t="s">
+      <c r="H59" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I59" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J59" s="20" t="s">
+      <c r="I59" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K59" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M59" s="20" t="s">
+      <c r="L59" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M59" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20829,16 +20830,16 @@
       <c r="A60" t="s">
         <v>700</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" s="20" t="s">
+      <c r="D60" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F60">
@@ -20847,22 +20848,22 @@
       <c r="G60" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H60" s="20" t="s">
+      <c r="H60" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I60" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J60" s="20" t="s">
+      <c r="I60" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J60" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K60" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L60" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M60" s="20" t="s">
+      <c r="L60" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M60" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20870,16 +20871,16 @@
       <c r="A61" t="s">
         <v>698</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F61">
@@ -20888,22 +20889,22 @@
       <c r="G61" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H61" s="20" t="s">
+      <c r="H61" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I61" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J61" s="20" t="s">
+      <c r="I61" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J61" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K61" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L61" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M61" s="20" t="s">
+      <c r="L61" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M61" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20911,16 +20912,16 @@
       <c r="A62" t="s">
         <v>696</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E62" s="20" t="s">
+      <c r="D62" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F62">
@@ -20929,22 +20930,22 @@
       <c r="G62" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="H62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I62" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J62" s="20" t="s">
+      <c r="I62" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J62" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K62" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L62" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M62" s="20" t="s">
+      <c r="L62" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M62" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20952,16 +20953,16 @@
       <c r="A63" t="s">
         <v>694</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F63">
@@ -20970,22 +20971,22 @@
       <c r="G63" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H63" s="20" t="s">
+      <c r="H63" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I63" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J63" s="20" t="s">
+      <c r="I63" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K63" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L63" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M63" s="20" t="s">
+      <c r="L63" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M63" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -20993,16 +20994,16 @@
       <c r="A64" t="s">
         <v>692</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E64" s="20" t="s">
+      <c r="D64" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F64">
@@ -21011,22 +21012,22 @@
       <c r="G64" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H64" s="20" t="s">
+      <c r="H64" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="I64" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J64" s="20" t="s">
+      <c r="I64" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J64" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K64" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L64" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M64" s="20" t="s">
+      <c r="L64" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M64" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21034,16 +21035,16 @@
       <c r="A65" t="s">
         <v>690</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E65" s="20" t="s">
+      <c r="D65" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E65" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F65">
@@ -21052,22 +21053,22 @@
       <c r="G65" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H65" s="20" t="s">
+      <c r="H65" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="I65" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65" s="20" t="s">
+      <c r="I65" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K65" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L65" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M65" s="20" t="s">
+      <c r="L65" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M65" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21075,16 +21076,16 @@
       <c r="A66" t="s">
         <v>688</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E66" s="20" t="s">
+      <c r="E66" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F66">
@@ -21093,22 +21094,22 @@
       <c r="G66" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H66" s="20" t="s">
+      <c r="H66" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="I66" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J66" s="20" t="s">
+      <c r="I66" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K66" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L66" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M66" s="20" t="s">
+      <c r="L66" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M66" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21116,16 +21117,16 @@
       <c r="A67" t="s">
         <v>686</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E67" s="20" t="s">
+      <c r="D67" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F67">
@@ -21134,22 +21135,22 @@
       <c r="G67" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H67" s="20" t="s">
+      <c r="H67" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I67" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J67" s="20" t="s">
+      <c r="I67" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L67" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M67" s="20" t="s">
+      <c r="L67" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M67" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21157,16 +21158,16 @@
       <c r="A68" t="s">
         <v>684</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E68" s="20" t="s">
+      <c r="D68" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E68" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F68">
@@ -21175,22 +21176,22 @@
       <c r="G68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H68" s="20" t="s">
+      <c r="H68" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="I68" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J68" s="20" t="s">
+      <c r="I68" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K68" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L68" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M68" s="20" t="s">
+      <c r="L68" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M68" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21198,16 +21199,16 @@
       <c r="A69" t="s">
         <v>682</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" s="20" t="s">
+      <c r="D69" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F69">
@@ -21216,22 +21217,22 @@
       <c r="G69" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H69" s="20" t="s">
+      <c r="H69" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="I69" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J69" s="20" t="s">
+      <c r="I69" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L69" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M69" s="20" t="s">
+      <c r="L69" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M69" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21239,16 +21240,16 @@
       <c r="A70" t="s">
         <v>680</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="20" t="s">
+      <c r="D70" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E70" s="20" t="s">
+      <c r="E70" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F70">
@@ -21257,22 +21258,22 @@
       <c r="G70" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H70" s="20" t="s">
+      <c r="H70" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I70" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J70" s="20" t="s">
+      <c r="I70" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J70" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L70" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M70" s="20" t="s">
+      <c r="L70" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M70" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21280,16 +21281,16 @@
       <c r="A71" t="s">
         <v>678</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E71" s="20" t="s">
+      <c r="D71" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E71" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F71">
@@ -21298,22 +21299,22 @@
       <c r="G71" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="I71" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J71" s="20" t="s">
+      <c r="I71" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J71" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L71" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M71" s="20" t="s">
+      <c r="L71" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M71" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21321,16 +21322,16 @@
       <c r="A72" t="s">
         <v>676</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D72" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F72">
@@ -21339,22 +21340,22 @@
       <c r="G72" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H72" s="20" t="s">
+      <c r="H72" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="I72" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J72" s="20" t="s">
+      <c r="I72" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J72" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K72" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L72" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M72" s="20" t="s">
+      <c r="L72" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M72" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21362,16 +21363,16 @@
       <c r="A73" t="s">
         <v>674</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D73" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E73" s="20" t="s">
+      <c r="D73" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F73">
@@ -21380,22 +21381,22 @@
       <c r="G73" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H73" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I73" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J73" s="20" t="s">
+      <c r="H73" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J73" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K73" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L73" s="20" t="s">
+      <c r="L73" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M73" s="20" t="s">
+      <c r="M73" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21403,16 +21404,16 @@
       <c r="A74" t="s">
         <v>672</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D74" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="E74" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F74">
@@ -21421,22 +21422,22 @@
       <c r="G74" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H74" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I74" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J74" s="20" t="s">
+      <c r="H74" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K74" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L74" s="20" t="s">
+      <c r="L74" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M74" s="20" t="s">
+      <c r="M74" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21444,16 +21445,16 @@
       <c r="A75" t="s">
         <v>670</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B75" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E75" s="20" t="s">
+      <c r="D75" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F75">
@@ -21462,22 +21463,22 @@
       <c r="G75" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H75" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I75" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J75" s="20" t="s">
+      <c r="H75" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I75" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J75" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K75" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L75" s="20" t="s">
+      <c r="L75" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M75" s="20" t="s">
+      <c r="M75" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21485,16 +21486,16 @@
       <c r="A76" t="s">
         <v>666</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E76" s="20" t="s">
+      <c r="E76" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F76">
@@ -21503,22 +21504,22 @@
       <c r="G76" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H76" s="20" t="s">
+      <c r="H76" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I76" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J76" s="20" t="s">
+      <c r="I76" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J76" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K76" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L76" s="20" t="s">
+      <c r="L76" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M76" s="20" t="s">
+      <c r="M76" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21526,16 +21527,16 @@
       <c r="A77" t="s">
         <v>668</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D77" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E77" s="20" t="s">
+      <c r="D77" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F77">
@@ -21544,22 +21545,22 @@
       <c r="G77" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H77" s="20" t="s">
+      <c r="H77" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="I77" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J77" s="20" t="s">
+      <c r="I77" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J77" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K77" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L77" s="20" t="s">
+      <c r="L77" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M77" s="20" t="s">
+      <c r="M77" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21567,16 +21568,16 @@
       <c r="A78" t="s">
         <v>664</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B78" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D78" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E78" s="20" t="s">
+      <c r="D78" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F78">
@@ -21585,22 +21586,22 @@
       <c r="G78" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H78" s="20" t="s">
+      <c r="H78" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="I78" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J78" s="20" t="s">
+      <c r="I78" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J78" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K78" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L78" s="20" t="s">
+      <c r="L78" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M78" s="20" t="s">
+      <c r="M78" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21608,16 +21609,16 @@
       <c r="A79" t="s">
         <v>662</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D79" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E79" s="20" t="s">
+      <c r="E79" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F79">
@@ -21626,22 +21627,22 @@
       <c r="G79" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H79" s="20" t="s">
+      <c r="H79" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="I79" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J79" s="20" t="s">
+      <c r="I79" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J79" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K79" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L79" s="20" t="s">
+      <c r="L79" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M79" s="20" t="s">
+      <c r="M79" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21649,16 +21650,16 @@
       <c r="A80" t="s">
         <v>660</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D80" s="20" t="s">
+      <c r="D80" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E80" s="20" t="s">
+      <c r="E80" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F80">
@@ -21667,22 +21668,22 @@
       <c r="G80" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H80" s="20" t="s">
+      <c r="H80" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I80" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J80" s="20" t="s">
+      <c r="I80" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J80" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K80" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L80" s="20" t="s">
+      <c r="L80" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M80" s="20" t="s">
+      <c r="M80" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21690,16 +21691,16 @@
       <c r="A81" t="s">
         <v>658</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="D81" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E81" s="20" t="s">
+      <c r="E81" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F81">
@@ -21708,22 +21709,22 @@
       <c r="G81" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H81" s="20" t="s">
+      <c r="H81" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="I81" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J81" s="20" t="s">
+      <c r="I81" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J81" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K81" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L81" s="20" t="s">
+      <c r="L81" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="M81" s="20" t="s">
+      <c r="M81" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21731,16 +21732,16 @@
       <c r="A82" t="s">
         <v>656</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B82" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E82" s="20" t="s">
+      <c r="D82" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="19" t="s">
         <v>197</v>
       </c>
       <c r="F82">
@@ -21749,22 +21750,22 @@
       <c r="G82" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H82" s="20" t="s">
+      <c r="H82" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="I82" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J82" s="20" t="s">
+      <c r="I82" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J82" s="19" t="s">
         <v>294</v>
       </c>
       <c r="K82" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L82" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M82" s="20" t="s">
+      <c r="L82" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M82" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21772,16 +21773,16 @@
       <c r="A83" t="s">
         <v>654</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C83" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D83" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E83" s="20" t="s">
+      <c r="D83" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F83">
@@ -21790,22 +21791,22 @@
       <c r="G83" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H83" s="20" t="s">
+      <c r="H83" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="I83" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J83" s="20" t="s">
+      <c r="I83" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J83" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K83" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L83" s="20" t="s">
+      <c r="L83" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="M83" s="20" t="s">
+      <c r="M83" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21813,16 +21814,16 @@
       <c r="A84" t="s">
         <v>652</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B84" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D84" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E84" s="20" t="s">
+      <c r="D84" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F84">
@@ -21831,22 +21832,22 @@
       <c r="G84" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H84" s="20" t="s">
+      <c r="H84" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="I84" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J84" s="20" t="s">
+      <c r="I84" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J84" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K84" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L84" s="20" t="s">
+      <c r="L84" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="M84" s="20" t="s">
+      <c r="M84" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21854,16 +21855,16 @@
       <c r="A85" t="s">
         <v>650</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D85" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E85" s="20" t="s">
+      <c r="D85" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F85">
@@ -21872,22 +21873,22 @@
       <c r="G85" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H85" s="20" t="s">
+      <c r="H85" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="I85" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J85" s="20" t="s">
+      <c r="I85" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J85" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K85" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L85" s="20" t="s">
+      <c r="L85" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="M85" s="20" t="s">
+      <c r="M85" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21895,16 +21896,16 @@
       <c r="A86" t="s">
         <v>648</v>
       </c>
-      <c r="B86" s="20" t="s">
+      <c r="B86" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D86" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E86" s="20" t="s">
+      <c r="D86" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F86">
@@ -21913,22 +21914,22 @@
       <c r="G86" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H86" s="20" t="s">
+      <c r="H86" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="I86" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J86" s="20" t="s">
+      <c r="I86" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J86" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K86" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L86" s="20" t="s">
+      <c r="L86" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="M86" s="20" t="s">
+      <c r="M86" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21936,16 +21937,16 @@
       <c r="A87" t="s">
         <v>646</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="B87" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D87" s="20" t="s">
+      <c r="D87" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E87" s="20" t="s">
+      <c r="E87" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F87">
@@ -21954,22 +21955,22 @@
       <c r="G87" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H87" s="20" t="s">
+      <c r="H87" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="I87" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J87" s="20" t="s">
+      <c r="I87" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J87" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K87" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L87" s="20" t="s">
+      <c r="L87" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M87" s="20" t="s">
+      <c r="M87" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -21977,16 +21978,16 @@
       <c r="A88" t="s">
         <v>644</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D88" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E88" s="20" t="s">
+      <c r="D88" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F88">
@@ -21995,22 +21996,22 @@
       <c r="G88" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H88" s="20" t="s">
+      <c r="H88" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I88" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J88" s="20" t="s">
+      <c r="I88" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J88" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K88" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L88" s="20" t="s">
+      <c r="L88" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M88" s="20" t="s">
+      <c r="M88" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22018,16 +22019,16 @@
       <c r="A89" t="s">
         <v>642</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D89" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E89" s="20" t="s">
+      <c r="D89" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F89">
@@ -22036,22 +22037,22 @@
       <c r="G89" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H89" s="20" t="s">
+      <c r="H89" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="I89" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J89" s="20" t="s">
+      <c r="I89" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J89" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K89" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L89" s="20" t="s">
+      <c r="L89" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M89" s="20" t="s">
+      <c r="M89" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22059,16 +22060,16 @@
       <c r="A90" t="s">
         <v>640</v>
       </c>
-      <c r="B90" s="20" t="s">
+      <c r="B90" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D90" s="20" t="s">
+      <c r="D90" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E90" s="20" t="s">
+      <c r="E90" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F90">
@@ -22077,22 +22078,22 @@
       <c r="G90" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H90" s="20" t="s">
+      <c r="H90" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="I90" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J90" s="20" t="s">
+      <c r="I90" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J90" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K90" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L90" s="20" t="s">
+      <c r="L90" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M90" s="20" t="s">
+      <c r="M90" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22100,16 +22101,16 @@
       <c r="A91" t="s">
         <v>638</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B91" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D91" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E91" s="20" t="s">
+      <c r="D91" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E91" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F91">
@@ -22118,22 +22119,22 @@
       <c r="G91" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H91" s="20" t="s">
+      <c r="H91" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I91" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J91" s="20" t="s">
+      <c r="I91" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J91" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K91" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L91" s="20" t="s">
+      <c r="L91" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M91" s="20" t="s">
+      <c r="M91" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22141,16 +22142,16 @@
       <c r="A92" t="s">
         <v>636</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="C92" s="20" t="s">
+      <c r="C92" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E92" s="20" t="s">
+      <c r="D92" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F92">
@@ -22159,22 +22160,22 @@
       <c r="G92" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H92" s="20" t="s">
+      <c r="H92" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="I92" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J92" s="20" t="s">
+      <c r="I92" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J92" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K92" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L92" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M92" s="20" t="s">
+      <c r="L92" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M92" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22182,16 +22183,16 @@
       <c r="A93" t="s">
         <v>634</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D93" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E93" s="20" t="s">
+      <c r="D93" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F93">
@@ -22200,22 +22201,22 @@
       <c r="G93" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H93" s="20" t="s">
+      <c r="H93" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="I93" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J93" s="20" t="s">
+      <c r="I93" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J93" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K93" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L93" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M93" s="20" t="s">
+      <c r="L93" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M93" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22223,16 +22224,16 @@
       <c r="A94" t="s">
         <v>632</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D94" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E94" s="20" t="s">
+      <c r="D94" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F94">
@@ -22241,22 +22242,22 @@
       <c r="G94" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H94" s="20" t="s">
+      <c r="H94" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="I94" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J94" s="20" t="s">
+      <c r="I94" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J94" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K94" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L94" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M94" s="20" t="s">
+      <c r="L94" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M94" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22264,16 +22265,16 @@
       <c r="A95" t="s">
         <v>630</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B95" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C95" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D95" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E95" s="20" t="s">
+      <c r="D95" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F95">
@@ -22282,22 +22283,22 @@
       <c r="G95" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H95" s="20" t="s">
+      <c r="H95" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="I95" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J95" s="20" t="s">
+      <c r="I95" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J95" s="19" t="s">
         <v>273</v>
       </c>
       <c r="K95" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L95" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M95" s="20" t="s">
+      <c r="L95" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M95" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22305,16 +22306,16 @@
       <c r="A96" t="s">
         <v>628</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C96" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D96" s="20" t="s">
+      <c r="D96" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E96" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F96">
@@ -22323,22 +22324,22 @@
       <c r="G96" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H96" s="20" t="s">
+      <c r="H96" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I96" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J96" s="20" t="s">
+      <c r="I96" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J96" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K96" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L96" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M96" s="20" t="s">
+      <c r="L96" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M96" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -22346,16 +22347,16 @@
       <c r="A97" t="s">
         <v>624</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D97" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E97" s="20" t="s">
+      <c r="D97" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F97">
@@ -22364,22 +22365,22 @@
       <c r="G97" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H97" s="20" t="s">
+      <c r="H97" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I97" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J97" s="20" t="s">
+      <c r="I97" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J97" s="19" t="s">
         <v>294</v>
       </c>
       <c r="K97" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L97" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M97" s="20" t="s">
+      <c r="L97" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M97" s="19" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>